<commit_message>
Grobplanung aktualisiert, Meilensteine komplettiert.
</commit_message>
<xml_diff>
--- a/doku/Grobplanung.xlsx
+++ b/doku/Grobplanung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19320" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>andjoy - Grobplanung</t>
   </si>
@@ -115,13 +115,22 @@
   </si>
   <si>
     <t>Iteration</t>
+  </si>
+  <si>
+    <t>Audio lokal abspeichern nicht praktikabel, zu wenig Speicher</t>
+  </si>
+  <si>
+    <t>accepted</t>
+  </si>
+  <si>
+    <t>Video lokal abspeichern nicht praktikabel, zu wenig Speicher, Video ohne Text einbinden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,14 +162,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -474,35 +509,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -510,58 +524,114 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -858,7 +928,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -872,7 +944,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
     </row>
@@ -940,354 +1012,370 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="18.75">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="16"/>
+      <c r="C12" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="26" t="s">
+      <c r="D12" s="20"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="28"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="21" t="s">
+      <c r="K13" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="9">
+    <row r="14" spans="1:11" s="27" customFormat="1">
+      <c r="A14" s="21">
         <v>1</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="23">
         <v>8</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="23">
         <f>B8*C14*B6</f>
         <v>24</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="24">
         <v>40834</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="24">
         <v>40862</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="23">
         <v>1</v>
       </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="35"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="12">
+      <c r="H14" s="24">
+        <v>40850</v>
+      </c>
+      <c r="I14" s="25">
+        <v>15</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="59" customFormat="1">
+      <c r="A15" s="57">
         <v>2</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
       <c r="I15" s="31"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="36"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="12">
+      <c r="J15" s="29"/>
+      <c r="K15" s="32"/>
+    </row>
+    <row r="16" spans="1:11" s="27" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A16" s="28">
         <v>3</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="34">
         <v>2</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="34">
         <f>C16*B8*B6</f>
         <v>6</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="35">
         <v>40864</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16" s="35">
         <v>40869</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="34">
         <v>2</v>
       </c>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="32"/>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="12">
+      <c r="H16" s="35">
+        <v>40850</v>
+      </c>
+      <c r="I16" s="34">
+        <v>15</v>
+      </c>
+      <c r="J16" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="36"/>
+    </row>
+    <row r="17" spans="1:11" s="43" customFormat="1">
+      <c r="A17" s="37">
         <v>4</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="39">
         <v>4</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="39">
         <f>C17*B8*B6</f>
         <v>12</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="40">
         <v>40871</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="40">
         <v>40883</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="39">
         <v>3</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="37"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="12">
+      <c r="H17" s="39"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="59" customFormat="1">
+      <c r="A18" s="57">
         <v>5</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="36"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="12">
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="45"/>
+    </row>
+    <row r="19" spans="1:11" s="43" customFormat="1">
+      <c r="A19" s="37">
         <v>6</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="39">
         <v>2</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="39">
         <f>C19*B8*B6</f>
         <v>6</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="40">
         <v>40885</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="40">
         <v>40890</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="39">
         <v>4</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="37"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="12">
+      <c r="H19" s="39"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="47"/>
+    </row>
+    <row r="20" spans="1:11" s="43" customFormat="1">
+      <c r="A20" s="37">
         <v>7</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="36"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="12">
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="48"/>
+    </row>
+    <row r="21" spans="1:11" s="43" customFormat="1">
+      <c r="A21" s="37">
         <v>8</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="49">
         <v>1</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="49">
         <f>$B$8*C21*$B$6</f>
         <v>3</v>
       </c>
-      <c r="E21" s="38">
+      <c r="E21" s="50">
         <v>40892</v>
       </c>
-      <c r="F21" s="38">
+      <c r="F21" s="50">
         <v>40892</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="49">
         <v>5</v>
       </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="32"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="12">
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="51"/>
+    </row>
+    <row r="22" spans="1:11" s="43" customFormat="1">
+      <c r="A22" s="37">
         <v>9</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="49">
         <v>1</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="49">
         <f t="shared" ref="D22:D24" si="0">$B$8*C22*$B$6</f>
         <v>3</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="50">
         <v>40897</v>
       </c>
-      <c r="F22" s="38">
+      <c r="F22" s="50">
         <v>40897</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="49">
         <v>6</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="32"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="12">
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="51"/>
+    </row>
+    <row r="23" spans="1:11" s="43" customFormat="1">
+      <c r="A23" s="37">
         <v>10</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="25">
+      <c r="C23" s="49">
         <v>2</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="49">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="50">
         <v>40899</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="50">
         <v>40918</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="49">
         <v>7</v>
       </c>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="32"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A24" s="7">
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="51"/>
+    </row>
+    <row r="24" spans="1:11" s="43" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A24" s="52">
         <v>11</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="29">
+      <c r="C24" s="54">
         <v>1</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="54">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E24" s="39">
+      <c r="E24" s="55">
         <v>40920</v>
       </c>
-      <c r="F24" s="39">
+      <c r="F24" s="55">
         <v>40920</v>
       </c>
-      <c r="G24" s="29">
+      <c r="G24" s="54">
         <v>8</v>
       </c>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="34"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="56"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1">
       <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" s="22">
+      <c r="C25" s="11">
         <f>SUM(C14:C24)</f>
         <v>21</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="11">
         <f>SUM(D14:D24)</f>
         <v>63</v>
       </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="23"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="2" t="s">
@@ -1297,13 +1385,27 @@
         <f>B5-C25</f>
         <v>3</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="13">
         <f>B9-D25</f>
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="K17:K18"/>
     <mergeCell ref="K19:K20"/>
@@ -1320,20 +1422,6 @@
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>